<commit_message>
Update Original File Explanation.xlsx
</commit_message>
<xml_diff>
--- a/docs/Original File Explanation.xlsx
+++ b/docs/Original File Explanation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbilley\Documents\GitHub\soip-workflow-automation\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416EA19B-8DA7-4BF5-B486-B5986311E966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BB24EC-AE01-4442-8874-262BD228BA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7830" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{1C6CA263-56D1-4D08-A1E7-314EDB8B9C74}"/>
+    <workbookView xWindow="28680" yWindow="-7830" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="12" xr2:uid="{1C6CA263-56D1-4D08-A1E7-314EDB8B9C74}"/>
   </bookViews>
   <sheets>
     <sheet name="High Level" sheetId="2" r:id="rId1"/>
@@ -28,6 +28,13 @@
     <sheet name="CF Tables Altered" sheetId="16" r:id="rId13"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'010-Depot Costs...'!$A$1:$E$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'015 - Set SOIP Solve Flag'!$A$1:$E$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'017 - Issue and Return...'!$A$1:$E$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'020 - Lane Attributes'!$A$1:$E$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'060 - Transportation Rates Hist'!$A$1:$E$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'070 - Trans Load Size'!$A$1:$E$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'090 - Flag Multi Source'!$A$1:$E$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'CF Tables Altered'!$A$1:$D$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Specific Files'!$B$1:$F$53</definedName>
   </definedNames>
@@ -52,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="774">
   <si>
     <t>Type</t>
   </si>
@@ -3413,6 +3420,9 @@
 UPDATE: All rows where bomname is blank is returns, and we aren't including a return cost.
 Why update [depottype] before and after the union?
 UPDATE: Can eliminate the first one.</t>
+  </si>
+  <si>
+    <t>This looks back 60 days. Other SQL Queries look back 90 days? (See Transportation Rates Hist)</t>
   </si>
 </sst>
 </file>
@@ -3594,7 +3604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3691,6 +3701,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4247,7 +4261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E843C-44E2-4B22-A3F0-78A006B486F1}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -5080,8 +5094,8 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5250,7 +5264,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="25" customFormat="1" ht="174" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" s="25" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
         <v>723</v>
       </c>
@@ -5275,7 +5289,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="27" customFormat="1" ht="261" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" s="27" customFormat="1" ht="290" x14ac:dyDescent="0.35">
       <c r="A17" s="27" t="s">
         <v>726</v>
       </c>
@@ -5344,7 +5358,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="30" customFormat="1" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" s="30" customFormat="1" ht="319" x14ac:dyDescent="0.35">
       <c r="A23" s="30" t="s">
         <v>721</v>
       </c>
@@ -5366,7 +5380,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="30" customFormat="1" ht="290" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" s="30" customFormat="1" ht="348" x14ac:dyDescent="0.35">
       <c r="A25" s="30" t="s">
         <v>721</v>
       </c>
@@ -5377,7 +5391,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="30" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" s="30" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A26" s="30" t="s">
         <v>721</v>
       </c>
@@ -5405,7 +5419,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="31" customFormat="1" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" s="31" customFormat="1" ht="319" x14ac:dyDescent="0.35">
       <c r="A28" s="31" t="s">
         <v>718</v>
       </c>
@@ -5444,10 +5458,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E49616A-EF6F-49EC-9DA2-E4B17497683E}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5474,7 +5489,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5483,7 +5498,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -5492,7 +5507,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -5501,7 +5516,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -5520,7 +5535,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>104</v>
       </c>
@@ -5531,12 +5546,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>89</v>
       </c>
@@ -5544,7 +5559,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>105</v>
       </c>
@@ -5555,17 +5570,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>106</v>
       </c>
@@ -5576,7 +5591,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>108</v>
       </c>
@@ -5588,7 +5603,7 @@
       </c>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D15" s="9" t="s">
         <v>219</v>
       </c>
@@ -5596,7 +5611,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>97</v>
       </c>
@@ -5604,17 +5619,17 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>107</v>
       </c>
@@ -5622,7 +5637,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B20" s="8" t="s">
         <v>130</v>
       </c>
@@ -5630,7 +5645,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>5</v>
       </c>
@@ -5649,7 +5664,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>104</v>
       </c>
@@ -5663,7 +5678,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D24" s="9" t="s">
         <v>113</v>
       </c>
@@ -5671,7 +5686,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>105</v>
       </c>
@@ -5682,17 +5697,18 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>106</v>
       </c>
@@ -5703,12 +5719,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D30" s="9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31" s="8" t="s">
         <v>108</v>
       </c>
@@ -5719,7 +5735,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>6</v>
       </c>
@@ -5738,7 +5754,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>104</v>
       </c>
@@ -5749,12 +5765,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>105</v>
       </c>
@@ -5765,7 +5781,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>106</v>
       </c>
@@ -5776,17 +5792,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="D38" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="D39" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>108</v>
       </c>
@@ -5797,7 +5813,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>107</v>
       </c>
@@ -5808,7 +5824,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>130</v>
       </c>
@@ -5819,7 +5835,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>141</v>
       </c>
@@ -5830,7 +5846,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>110</v>
       </c>
@@ -5841,17 +5857,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="D45" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="D46" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B47" s="8" t="s">
         <v>148</v>
       </c>
@@ -5866,7 +5882,7 @@
       </c>
       <c r="F47" s="10"/>
     </row>
-    <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>7</v>
       </c>
@@ -5885,7 +5901,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>104</v>
       </c>
@@ -5896,7 +5912,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>105</v>
       </c>
@@ -5907,17 +5923,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D52" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D53" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>106</v>
       </c>
@@ -5928,7 +5944,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>108</v>
       </c>
@@ -5939,7 +5955,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B56" s="8" t="s">
         <v>107</v>
       </c>
@@ -5950,7 +5966,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>8</v>
       </c>
@@ -5980,7 +5996,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>105</v>
       </c>
@@ -5988,7 +6004,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>106</v>
       </c>
@@ -5999,17 +6015,17 @@
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D62" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D63" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>108</v>
       </c>
@@ -6020,17 +6036,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D65" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D66" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>107</v>
       </c>
@@ -6041,12 +6057,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D68" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>130</v>
       </c>
@@ -6057,7 +6073,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="70" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B70" s="8" t="s">
         <v>141</v>
       </c>
@@ -6068,7 +6084,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>9</v>
       </c>
@@ -6087,7 +6103,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>104</v>
       </c>
@@ -6098,7 +6114,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>105</v>
       </c>
@@ -6109,7 +6125,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>106</v>
       </c>
@@ -6120,17 +6136,17 @@
         <v>185</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D76" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D77" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>108</v>
       </c>
@@ -6141,12 +6157,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D79" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>107</v>
       </c>
@@ -6157,17 +6173,17 @@
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D81" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D82" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>130</v>
       </c>
@@ -6178,12 +6194,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D84" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>141</v>
       </c>
@@ -6194,7 +6210,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>110</v>
       </c>
@@ -6205,7 +6221,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>148</v>
       </c>
@@ -6216,17 +6232,17 @@
         <v>189</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D88" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D89" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>190</v>
       </c>
@@ -6237,7 +6253,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="91" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B91" s="8" t="s">
         <v>191</v>
       </c>
@@ -6248,7 +6264,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>10</v>
       </c>
@@ -6267,7 +6283,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>104</v>
       </c>
@@ -6278,7 +6294,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>105</v>
       </c>
@@ -6289,17 +6305,17 @@
         <v>196</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D96" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D97" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>106</v>
       </c>
@@ -6310,17 +6326,17 @@
         <v>199</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D99" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D100" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>108</v>
       </c>
@@ -6331,12 +6347,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D102" s="6" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>107</v>
       </c>
@@ -6347,7 +6363,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="104" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B104" s="8" t="s">
         <v>130</v>
       </c>
@@ -6358,7 +6374,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>11</v>
       </c>
@@ -6377,7 +6393,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>104</v>
       </c>
@@ -6388,17 +6404,17 @@
         <v>211</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D108" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D109" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>105</v>
       </c>
@@ -6409,17 +6425,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D111" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D112" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>106</v>
       </c>
@@ -6430,12 +6446,12 @@
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D114" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="115" spans="2:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:4" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B115" s="8" t="s">
         <v>108</v>
       </c>
@@ -6446,20 +6462,29 @@
         <v>218</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:4" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="117" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B117" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E117" xr:uid="{6E49616A-EF6F-49EC-9DA2-E4B17497683E}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Execute the following SQL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874C9A7F-8056-4B55-BD1C-FF48D0F05B92}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6487,7 +6512,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -6496,7 +6521,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -6511,7 +6536,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -6541,7 +6566,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>105</v>
       </c>
@@ -6552,7 +6577,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>106</v>
       </c>
@@ -6563,7 +6588,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>108</v>
       </c>
@@ -6574,17 +6599,17 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>107</v>
       </c>
@@ -6595,7 +6620,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" s="8" t="s">
         <v>130</v>
       </c>
@@ -6606,7 +6631,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -6636,7 +6661,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>105</v>
       </c>
@@ -6647,7 +6672,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>106</v>
       </c>
@@ -6658,7 +6683,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>108</v>
       </c>
@@ -6669,7 +6694,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>107</v>
       </c>
@@ -6680,17 +6705,17 @@
         <v>234</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>130</v>
       </c>
@@ -6701,7 +6726,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B24" s="8" t="s">
         <v>141</v>
       </c>
@@ -6712,7 +6737,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -6720,7 +6745,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -6729,7 +6754,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>7</v>
       </c>
@@ -6738,7 +6763,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>8</v>
       </c>
@@ -6757,7 +6782,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>104</v>
       </c>
@@ -6768,7 +6793,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>105</v>
       </c>
@@ -6779,7 +6804,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>106</v>
       </c>
@@ -6790,7 +6815,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>108</v>
       </c>
@@ -6801,7 +6826,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>107</v>
       </c>
@@ -6812,7 +6837,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" s="8" t="s">
         <v>130</v>
       </c>
@@ -6823,7 +6848,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>9</v>
       </c>
@@ -6842,7 +6867,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>104</v>
       </c>
@@ -6853,7 +6878,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>105</v>
       </c>
@@ -6864,7 +6889,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>106</v>
       </c>
@@ -6875,7 +6900,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>108</v>
       </c>
@@ -6886,7 +6911,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>107</v>
       </c>
@@ -6897,7 +6922,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B43" s="8" t="s">
         <v>130</v>
       </c>
@@ -6909,6 +6934,18 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E43" xr:uid="{874C9A7F-8056-4B55-BD1C-FF48D0F05B92}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Customer demand - Execute the following SQL"/>
+        <filter val="Customer fulfillment policies in model - Execute the following SQL"/>
+        <filter val="Customer table in model - Execute the following SQL"/>
+        <filter val="Facilities table in model - Execute the following SQL"/>
+        <filter val="Replenishment policies table in model - Execute the following SQL"/>
+        <filter val="Return forecast - Execute the following SQL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -6916,10 +6953,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066D2980-1350-49EA-B629-4EB5DB48219D}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6954,14 +6992,14 @@
       <c r="C2" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="49" t="s">
         <v>268</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -6980,7 +7018,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>104</v>
       </c>
@@ -6991,7 +7029,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>105</v>
       </c>
@@ -7002,7 +7040,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>106</v>
       </c>
@@ -7013,17 +7051,17 @@
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>108</v>
       </c>
@@ -7034,7 +7072,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>107</v>
       </c>
@@ -7045,7 +7083,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>130</v>
       </c>
@@ -7056,7 +7094,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>141</v>
       </c>
@@ -7067,17 +7105,17 @@
         <v>280</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>110</v>
       </c>
@@ -7088,7 +7126,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B17" s="8" t="s">
         <v>148</v>
       </c>
@@ -7099,7 +7137,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>3</v>
       </c>
@@ -7108,7 +7146,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
         <v>4</v>
       </c>
@@ -7119,7 +7157,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>5</v>
       </c>
@@ -7127,7 +7165,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>103</v>
       </c>
@@ -7149,7 +7187,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>105</v>
       </c>
@@ -7160,7 +7198,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>106</v>
       </c>
@@ -7174,7 +7212,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>108</v>
       </c>
@@ -7185,17 +7223,17 @@
         <v>289</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>107</v>
       </c>
@@ -7206,7 +7244,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>130</v>
       </c>
@@ -7217,7 +7255,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>141</v>
       </c>
@@ -7228,7 +7266,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>110</v>
       </c>
@@ -7239,17 +7277,17 @@
         <v>298</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:4" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>148</v>
       </c>
@@ -7260,7 +7298,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>190</v>
       </c>
@@ -7271,7 +7309,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:4" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>191</v>
       </c>
@@ -7282,7 +7320,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="37" spans="2:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:4" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B37" s="8" t="s">
         <v>304</v>
       </c>
@@ -7294,6 +7332,15 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E37" xr:uid="{066D2980-1350-49EA-B629-4EB5DB48219D}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Customer table in model - Execute the following SQL"/>
+        <filter val="Location table in data warehouse - Execute the following SQL"/>
+        <filter val="Return forecast - Execute the following SQL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -7301,10 +7348,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A45E050-E71B-4380-9782-9CB2A1906CE4}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7339,11 +7387,11 @@
       <c r="C2" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="50" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -7354,7 +7402,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -7365,7 +7413,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -7376,7 +7424,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -7387,7 +7435,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -7398,17 +7446,17 @@
         <v>313</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -7419,7 +7467,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -7430,17 +7478,17 @@
         <v>317</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -7451,7 +7499,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -7462,7 +7510,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>11</v>
       </c>
@@ -7473,7 +7521,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -7492,7 +7540,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>104</v>
       </c>
@@ -7506,19 +7554,19 @@
         <v>368</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>326</v>
       </c>
       <c r="E20" s="45"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
         <v>328</v>
       </c>
       <c r="E21" s="45"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>105</v>
       </c>
@@ -7530,7 +7578,7 @@
       </c>
       <c r="E22" s="45"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>106</v>
       </c>
@@ -7542,19 +7590,19 @@
       </c>
       <c r="E23" s="45"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
         <v>333</v>
       </c>
       <c r="E24" s="45"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D25" t="s">
         <v>334</v>
       </c>
       <c r="E25" s="45"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>108</v>
       </c>
@@ -7577,7 +7625,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>130</v>
       </c>
@@ -7588,7 +7636,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>141</v>
       </c>
@@ -7599,7 +7647,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>110</v>
       </c>
@@ -7610,7 +7658,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>148</v>
       </c>
@@ -7621,17 +7669,17 @@
         <v>339</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="261" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>190</v>
       </c>
@@ -7642,7 +7690,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>191</v>
       </c>
@@ -7653,17 +7701,17 @@
         <v>344</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D37" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>304</v>
       </c>
@@ -7677,7 +7725,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B39" s="8" t="s">
         <v>350</v>
       </c>
@@ -7688,7 +7736,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>13</v>
       </c>
@@ -7697,7 +7745,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="8">
         <v>14</v>
       </c>
@@ -7708,7 +7756,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>15</v>
       </c>
@@ -7727,7 +7775,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>104</v>
       </c>
@@ -7741,19 +7789,19 @@
         <v>368</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D45" t="s">
         <v>355</v>
       </c>
       <c r="E45" s="45"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D46" t="s">
         <v>334</v>
       </c>
       <c r="E46" s="45"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>105</v>
       </c>
@@ -7765,7 +7813,7 @@
       </c>
       <c r="E47" s="45"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>106</v>
       </c>
@@ -7777,19 +7825,19 @@
       </c>
       <c r="E48" s="45"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D49" t="s">
         <v>333</v>
       </c>
       <c r="E49" s="45"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D50" t="s">
         <v>334</v>
       </c>
       <c r="E50" s="45"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>108</v>
       </c>
@@ -7812,7 +7860,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>130</v>
       </c>
@@ -7823,7 +7871,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>141</v>
       </c>
@@ -7834,7 +7882,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="55" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>110</v>
       </c>
@@ -7845,7 +7893,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>148</v>
       </c>
@@ -7856,17 +7904,17 @@
         <v>366</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D57" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D58" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5" ht="246.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>190</v>
       </c>
@@ -7877,7 +7925,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>191</v>
       </c>
@@ -7888,17 +7936,17 @@
         <v>370</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D61" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D62" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="63" spans="2:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>304</v>
       </c>
@@ -7909,7 +7957,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="64" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B64" s="8" t="s">
         <v>350</v>
       </c>
@@ -7920,7 +7968,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>16</v>
       </c>
@@ -7939,7 +7987,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>104</v>
       </c>
@@ -7950,17 +7998,17 @@
         <v>376</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D68" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D69" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>105</v>
       </c>
@@ -7971,7 +8019,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>106</v>
       </c>
@@ -7982,17 +8030,17 @@
         <v>379</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D72" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D73" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>108</v>
       </c>
@@ -8003,7 +8051,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>107</v>
       </c>
@@ -8014,7 +8062,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B76" s="8" t="s">
         <v>130</v>
       </c>
@@ -8025,7 +8073,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>17</v>
       </c>
@@ -8034,7 +8082,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="B78" s="13" t="s">
         <v>103</v>
       </c>
@@ -8048,7 +8096,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B79" s="13" t="s">
         <v>104</v>
       </c>
@@ -8060,7 +8108,7 @@
       </c>
       <c r="E79" s="46"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B80" s="13" t="s">
         <v>105</v>
       </c>
@@ -8072,7 +8120,7 @@
       </c>
       <c r="E80" s="46"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B81" s="13" t="s">
         <v>106</v>
       </c>
@@ -8084,7 +8132,7 @@
       </c>
       <c r="E81" s="46"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B82" s="13" t="s">
         <v>108</v>
       </c>
@@ -8096,7 +8144,7 @@
       </c>
       <c r="E82" s="46"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B83" s="13" t="s">
         <v>107</v>
       </c>
@@ -8108,7 +8156,7 @@
       </c>
       <c r="E83" s="46"/>
     </row>
-    <row r="84" spans="2:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:5" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B84" s="13" t="s">
         <v>130</v>
       </c>
@@ -8120,7 +8168,7 @@
       </c>
       <c r="E84" s="46"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B85" s="13" t="s">
         <v>141</v>
       </c>
@@ -8132,7 +8180,7 @@
       </c>
       <c r="E85" s="46"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B86" s="13" t="s">
         <v>110</v>
       </c>
@@ -8144,7 +8192,7 @@
       </c>
       <c r="E86" s="46"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B87" s="13" t="s">
         <v>148</v>
       </c>
@@ -8156,7 +8204,7 @@
       </c>
       <c r="E87" s="46"/>
     </row>
-    <row r="88" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:5" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="B88" s="15" t="s">
         <v>190</v>
       </c>
@@ -8170,7 +8218,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B89" s="15" t="s">
         <v>191</v>
       </c>
@@ -8182,7 +8230,7 @@
       </c>
       <c r="E89" s="47"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B90" s="15" t="s">
         <v>304</v>
       </c>
@@ -8194,7 +8242,7 @@
       </c>
       <c r="E90" s="47"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B91" s="15" t="s">
         <v>350</v>
       </c>
@@ -8206,7 +8254,7 @@
       </c>
       <c r="E91" s="47"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B92" s="15" t="s">
         <v>402</v>
       </c>
@@ -8218,7 +8266,7 @@
       </c>
       <c r="E92" s="47"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B93" s="15" t="s">
         <v>403</v>
       </c>
@@ -8230,7 +8278,7 @@
       </c>
       <c r="E93" s="47"/>
     </row>
-    <row r="94" spans="2:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:5" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B94" s="15" t="s">
         <v>404</v>
       </c>
@@ -8242,7 +8290,7 @@
       </c>
       <c r="E94" s="47"/>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B95" s="15" t="s">
         <v>405</v>
       </c>
@@ -8254,7 +8302,7 @@
       </c>
       <c r="E95" s="47"/>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B96" s="15" t="s">
         <v>406</v>
       </c>
@@ -8266,7 +8314,7 @@
       </c>
       <c r="E96" s="47"/>
     </row>
-    <row r="97" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B97" s="17" t="s">
         <v>407</v>
       </c>
@@ -8279,6 +8327,18 @@
       <c r="E97" s="47"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E97" xr:uid="{6A45E050-E71B-4380-9782-9CB2A1906CE4}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Customer demand - Execute the following SQL"/>
+        <filter val="Customer fulfillment policies table in model - Execute the following SQL"/>
+        <filter val="Issues from Data Warehouse - Execute the following SQL"/>
+        <filter val="Replenishment policies table in model - Execute the following SQL"/>
+        <filter val="Return forecast - Execute the following SQL"/>
+        <filter val="transportation policies table in model - Execute the following SQL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="4">
     <mergeCell ref="E19:E26"/>
     <mergeCell ref="E44:E51"/>
@@ -8294,7 +8354,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8465,10 +8525,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F333EE-53F3-4E6E-9E60-69C64448E149}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8507,7 +8568,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -8525,7 +8586,7 @@
       <c r="C4" t="s">
         <v>451</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="50" t="s">
         <v>450</v>
       </c>
     </row>
@@ -8551,7 +8612,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -8559,7 +8620,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>103</v>
       </c>
@@ -8570,7 +8631,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>104</v>
       </c>
@@ -8581,7 +8642,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>105</v>
       </c>
@@ -8592,7 +8653,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>106</v>
       </c>
@@ -8606,7 +8667,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>108</v>
       </c>
@@ -8617,7 +8678,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>107</v>
       </c>
@@ -8628,7 +8689,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>130</v>
       </c>
@@ -8642,19 +8703,19 @@
         <v>475</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>465</v>
       </c>
       <c r="E15" s="45"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>466</v>
       </c>
       <c r="E16" s="45"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>141</v>
       </c>
@@ -8666,19 +8727,19 @@
       </c>
       <c r="E17" s="45"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>468</v>
       </c>
       <c r="E18" s="45"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>469</v>
       </c>
       <c r="E19" s="45"/>
     </row>
-    <row r="20" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>110</v>
       </c>
@@ -8690,7 +8751,7 @@
       </c>
       <c r="E20" s="45"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>148</v>
       </c>
@@ -8702,7 +8763,7 @@
       </c>
       <c r="E21" s="45"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>190</v>
       </c>
@@ -8714,19 +8775,19 @@
       </c>
       <c r="E22" s="45"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
         <v>477</v>
       </c>
       <c r="E23" s="45"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
         <v>478</v>
       </c>
       <c r="E24" s="45"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>191</v>
       </c>
@@ -8738,19 +8799,19 @@
       </c>
       <c r="E25" s="45"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>480</v>
       </c>
       <c r="E26" s="45"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>481</v>
       </c>
       <c r="E27" s="45"/>
     </row>
-    <row r="28" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>304</v>
       </c>
@@ -8762,7 +8823,7 @@
       </c>
       <c r="E28" s="45"/>
     </row>
-    <row r="29" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>350</v>
       </c>
@@ -8774,7 +8835,7 @@
       </c>
       <c r="E29" s="45"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>402</v>
       </c>
@@ -8786,19 +8847,19 @@
       </c>
       <c r="E30" s="45"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D31" t="s">
         <v>480</v>
       </c>
       <c r="E31" s="45"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>481</v>
       </c>
       <c r="E32" s="45"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>403</v>
       </c>
@@ -8810,19 +8871,19 @@
       </c>
       <c r="E33" s="45"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D34" t="s">
         <v>480</v>
       </c>
       <c r="E34" s="45"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>481</v>
       </c>
       <c r="E35" s="45"/>
     </row>
-    <row r="36" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>404</v>
       </c>
@@ -8834,7 +8895,7 @@
       </c>
       <c r="E36" s="45"/>
     </row>
-    <row r="37" spans="1:5" s="8" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" s="8" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B37" s="8" t="s">
         <v>405</v>
       </c>
@@ -8846,7 +8907,7 @@
       </c>
       <c r="E37" s="45"/>
     </row>
-    <row r="38" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>7</v>
       </c>
@@ -8862,12 +8923,12 @@
       <c r="C39" t="s">
         <v>491</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="50" t="s">
         <v>492</v>
       </c>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>104</v>
       </c>
@@ -8879,7 +8940,7 @@
       </c>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>105</v>
       </c>
@@ -8893,7 +8954,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>106</v>
       </c>
@@ -8905,7 +8966,7 @@
       </c>
       <c r="E42" s="48"/>
     </row>
-    <row r="43" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>108</v>
       </c>
@@ -8917,7 +8978,7 @@
       </c>
       <c r="E43" s="48"/>
     </row>
-    <row r="44" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>107</v>
       </c>
@@ -8928,7 +8989,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>130</v>
       </c>
@@ -8939,7 +9000,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>141</v>
       </c>
@@ -8950,7 +9011,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>110</v>
       </c>
@@ -8961,7 +9022,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>148</v>
       </c>
@@ -8972,7 +9033,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>190</v>
       </c>
@@ -8983,7 +9044,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>191</v>
       </c>
@@ -8997,7 +9058,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="8" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" s="8" customFormat="1" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B51" s="8" t="s">
         <v>304</v>
       </c>
@@ -9008,7 +9069,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>8</v>
       </c>
@@ -9017,7 +9078,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>103</v>
       </c>
@@ -9031,7 +9092,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>104</v>
       </c>
@@ -9043,7 +9104,7 @@
       </c>
       <c r="E54" s="45"/>
     </row>
-    <row r="55" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>105</v>
       </c>
@@ -9055,7 +9116,7 @@
       </c>
       <c r="E55" s="45"/>
     </row>
-    <row r="56" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>106</v>
       </c>
@@ -9067,7 +9128,7 @@
       </c>
       <c r="E56" s="45"/>
     </row>
-    <row r="57" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>108</v>
       </c>
@@ -9079,7 +9140,7 @@
       </c>
       <c r="E57" s="45"/>
     </row>
-    <row r="58" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>107</v>
       </c>
@@ -9091,7 +9152,7 @@
       </c>
       <c r="E58" s="45"/>
     </row>
-    <row r="59" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>130</v>
       </c>
@@ -9103,7 +9164,7 @@
       </c>
       <c r="E59" s="45"/>
     </row>
-    <row r="60" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>141</v>
       </c>
@@ -9115,7 +9176,7 @@
       </c>
       <c r="E60" s="45"/>
     </row>
-    <row r="61" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>110</v>
       </c>
@@ -9127,7 +9188,7 @@
       </c>
       <c r="E61" s="45"/>
     </row>
-    <row r="62" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>148</v>
       </c>
@@ -9139,7 +9200,7 @@
       </c>
       <c r="E62" s="45"/>
     </row>
-    <row r="63" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>190</v>
       </c>
@@ -9151,7 +9212,7 @@
       </c>
       <c r="E63" s="45"/>
     </row>
-    <row r="64" spans="1:5" s="8" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" s="8" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B64" s="8" t="s">
         <v>191</v>
       </c>
@@ -9163,7 +9224,7 @@
       </c>
       <c r="E64" s="45"/>
     </row>
-    <row r="65" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>9</v>
       </c>
@@ -9171,7 +9232,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>103</v>
       </c>
@@ -9182,7 +9243,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>104</v>
       </c>
@@ -9193,7 +9254,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>105</v>
       </c>
@@ -9204,7 +9265,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>106</v>
       </c>
@@ -9215,7 +9276,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>108</v>
       </c>
@@ -9229,7 +9290,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>107</v>
       </c>
@@ -9243,7 +9304,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>130</v>
       </c>
@@ -9254,7 +9315,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>141</v>
       </c>
@@ -9265,7 +9326,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B74" s="8" t="s">
         <v>110</v>
       </c>
@@ -9276,7 +9337,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>10</v>
       </c>
@@ -9284,7 +9345,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>103</v>
       </c>
@@ -9295,7 +9356,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>104</v>
       </c>
@@ -9303,7 +9364,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>105</v>
       </c>
@@ -9317,7 +9378,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="8" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" s="8" customFormat="1" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="B79" s="8" t="s">
         <v>106</v>
       </c>
@@ -9328,7 +9389,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>11</v>
       </c>
@@ -9360,7 +9421,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>12</v>
       </c>
@@ -9369,7 +9430,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>103</v>
       </c>
@@ -9380,7 +9441,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>104</v>
       </c>
@@ -9391,7 +9452,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>105</v>
       </c>
@@ -9402,7 +9463,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>106</v>
       </c>
@@ -9413,7 +9474,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>108</v>
       </c>
@@ -9424,7 +9485,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>107</v>
       </c>
@@ -9435,7 +9496,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>130</v>
       </c>
@@ -9446,7 +9507,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>141</v>
       </c>
@@ -9457,7 +9518,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>110</v>
       </c>
@@ -9468,7 +9529,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>148</v>
       </c>
@@ -9479,7 +9540,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>190</v>
       </c>
@@ -9490,7 +9551,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>191</v>
       </c>
@@ -9501,7 +9562,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>304</v>
       </c>
@@ -9512,7 +9573,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>350</v>
       </c>
@@ -9523,7 +9584,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="98" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:4" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>402</v>
       </c>
@@ -9534,7 +9595,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="99" spans="2:4" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:4" s="8" customFormat="1" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B99" s="8" t="s">
         <v>403</v>
       </c>
@@ -9546,6 +9607,19 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E99" xr:uid="{82F333EE-53F3-4E6E-9E60-69C64448E149}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Customer table in model - Execute SQL"/>
+        <filter val="Data Warehouse - Count of loads by type and lane - Execute SQL"/>
+        <filter val="Data warehouse - Execute SQL"/>
+        <filter val="Facilities table in model - Execute SQL"/>
+        <filter val="Pull Customer Fulfillment Policies - Execute SQL"/>
+        <filter val="Pull Replenishment Policies - Execute SQL"/>
+        <filter val="Transportation Policies - Execute the following SQL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="E14:E37"/>
     <mergeCell ref="E41:E43"/>
@@ -9558,10 +9632,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44E2C992-6BA6-4B1E-BE92-1F54094E6342}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9589,7 +9664,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -9604,10 +9679,12 @@
       <c r="C3" t="s">
         <v>449</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="50" t="s">
         <v>576</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="20" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -9642,7 +9719,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -9651,7 +9728,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>103</v>
       </c>
@@ -9662,7 +9739,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>104</v>
       </c>
@@ -9673,7 +9750,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>105</v>
       </c>
@@ -9684,7 +9761,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>106</v>
       </c>
@@ -9695,7 +9772,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>108</v>
       </c>
@@ -9706,7 +9783,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>107</v>
       </c>
@@ -9717,7 +9794,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B14" s="8" t="s">
         <v>130</v>
       </c>
@@ -9731,7 +9808,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -9740,7 +9817,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>103</v>
       </c>
@@ -9751,7 +9828,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>104</v>
       </c>
@@ -9762,7 +9839,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>105</v>
       </c>
@@ -9773,7 +9850,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>106</v>
       </c>
@@ -9787,7 +9864,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>108</v>
       </c>
@@ -9798,7 +9875,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>107</v>
       </c>
@@ -9809,7 +9886,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>130</v>
       </c>
@@ -9820,7 +9897,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>141</v>
       </c>
@@ -9831,7 +9908,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>110</v>
       </c>
@@ -9842,7 +9919,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>148</v>
       </c>
@@ -9853,7 +9930,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="26" spans="2:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" s="8" customFormat="1" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B26" s="8" t="s">
         <v>190</v>
       </c>
@@ -9865,16 +9942,27 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E26" xr:uid="{44E2C992-6BA6-4B1E-BE92-1F54094E6342}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Customer table in model - Execute SQL"/>
+        <filter val="Data Warehouse - Execute SQL"/>
+        <filter val="Facilities table in model - Execute SQL"/>
+        <filter val="Transportation Policies table in model - Execute SQL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99BC76D-64B5-4D5F-A0C0-BCB3A903459D}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9902,7 +9990,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9910,7 +9998,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>103</v>
       </c>
@@ -9918,7 +10006,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>104</v>
       </c>
@@ -9940,7 +10028,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>106</v>
       </c>
@@ -9951,7 +10039,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>108</v>
       </c>
@@ -9962,7 +10050,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>107</v>
       </c>
@@ -9973,7 +10061,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>130</v>
       </c>
@@ -9984,7 +10072,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>141</v>
       </c>
@@ -9995,7 +10083,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>110</v>
       </c>
@@ -10009,7 +10097,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>148</v>
       </c>
@@ -10020,7 +10108,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" s="8" t="s">
         <v>190</v>
       </c>
@@ -10031,7 +10119,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
@@ -10050,7 +10138,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>104</v>
       </c>
@@ -10072,7 +10160,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>106</v>
       </c>
@@ -10083,7 +10171,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>108</v>
       </c>
@@ -10094,7 +10182,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>107</v>
       </c>
@@ -10105,7 +10193,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>130</v>
       </c>
@@ -10116,7 +10204,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>141</v>
       </c>
@@ -10127,7 +10215,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>110</v>
       </c>
@@ -10138,7 +10226,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>148</v>
       </c>
@@ -10149,7 +10237,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>190</v>
       </c>
@@ -10160,7 +10248,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>191</v>
       </c>
@@ -10171,7 +10259,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>304</v>
       </c>
@@ -10182,7 +10270,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>350</v>
       </c>
@@ -10193,7 +10281,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:4" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>402</v>
       </c>
@@ -10204,7 +10292,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>403</v>
       </c>
@@ -10215,7 +10303,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:4" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>404</v>
       </c>
@@ -10226,7 +10314,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>405</v>
       </c>
@@ -10237,7 +10325,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>406</v>
       </c>
@@ -10248,7 +10336,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="217.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>407</v>
       </c>
@@ -10262,7 +10350,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>613</v>
       </c>
@@ -10273,7 +10361,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>614</v>
       </c>
@@ -10284,7 +10372,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>615</v>
       </c>
@@ -10295,7 +10383,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" s="8" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B38" s="8" t="s">
         <v>616</v>
       </c>
@@ -10306,7 +10394,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>3</v>
       </c>
@@ -10314,7 +10402,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>103</v>
       </c>
@@ -10325,7 +10413,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>104</v>
       </c>
@@ -10336,7 +10424,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>105</v>
       </c>
@@ -10347,7 +10435,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>106</v>
       </c>
@@ -10358,7 +10446,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>108</v>
       </c>
@@ -10369,7 +10457,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>107</v>
       </c>
@@ -10383,7 +10471,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>130</v>
       </c>
@@ -10394,7 +10482,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>141</v>
       </c>
@@ -10405,7 +10493,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>110</v>
       </c>
@@ -10416,7 +10504,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>148</v>
       </c>
@@ -10438,7 +10526,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>191</v>
       </c>
@@ -10449,7 +10537,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>304</v>
       </c>
@@ -10463,7 +10551,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>350</v>
       </c>
@@ -10474,7 +10562,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>402</v>
       </c>
@@ -10488,7 +10576,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="55" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B55" s="8" t="s">
         <v>403</v>
       </c>
@@ -10500,6 +10588,16 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E55" xr:uid="{B99BC76D-64B5-4D5F-A0C0-BCB3A903459D}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Customer fulfilllment policies in table - Execute SQL"/>
+        <filter val="Customer table in model - Execute SQL"/>
+        <filter val="Group table in model - Execute SQL"/>
+        <filter val="Replenishment policies table in model - Execute SQL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>